<commit_message>
Agrego parciales de PN
</commit_message>
<xml_diff>
--- a/Parciales/Parcial1/ej1Parcial1.xlsx
+++ b/Parciales/Parcial1/ej1Parcial1.xlsx
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -252,6 +252,12 @@
     </xf>
     <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -869,10 +875,10 @@
       <c r="AI5" s="5"/>
       <c r="AJ5" s="5"/>
       <c r="AK5" s="3">
-        <v>14.0</v>
+        <v>16.0</v>
       </c>
       <c r="AL5" s="3">
-        <v>6.0</v>
+        <v>8.0</v>
       </c>
     </row>
     <row r="6">
@@ -894,7 +900,7 @@
       <c r="H6" s="6">
         <v>4.0</v>
       </c>
-      <c r="I6" s="6"/>
+      <c r="I6" s="3"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
@@ -923,12 +929,12 @@
       <c r="AI6" s="5"/>
       <c r="AJ6" s="5"/>
       <c r="AK6" s="5">
-        <f t="shared" ref="AK6:AL6" si="1">AVERAGE(AK2:AK5)</f>
-        <v>22.75</v>
+        <f>AVERAGE(AK2:AK5)</f>
+        <v>23.25</v>
       </c>
       <c r="AL6" s="5">
-        <f t="shared" si="1"/>
-        <v>15.25</v>
+        <f> AVERAGE(AL2:AL5)</f>
+        <v>15.75</v>
       </c>
     </row>
     <row r="7">
@@ -1675,6 +1681,125 @@
         <v>51</v>
       </c>
     </row>
+    <row r="71">
+      <c r="D71" s="2"/>
+    </row>
+    <row r="72">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="R72" s="1"/>
+      <c r="S72" s="1"/>
+      <c r="T72" s="1"/>
+      <c r="U72" s="1"/>
+      <c r="V72" s="1"/>
+      <c r="W72" s="1"/>
+      <c r="X72" s="1"/>
+      <c r="Y72" s="1"/>
+      <c r="AB72" s="1"/>
+      <c r="AC72" s="1"/>
+      <c r="AD72" s="1"/>
+      <c r="AE72" s="1"/>
+      <c r="AK72" s="1"/>
+      <c r="AL72" s="1"/>
+    </row>
+    <row r="73">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="Z73" s="1"/>
+      <c r="AA73" s="1"/>
+      <c r="AK73" s="1"/>
+      <c r="AL73" s="1"/>
+    </row>
+    <row r="74">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="AF74" s="1"/>
+      <c r="AG74" s="1"/>
+      <c r="AH74" s="1"/>
+      <c r="AI74" s="1"/>
+      <c r="AK74" s="1"/>
+      <c r="AL74" s="1"/>
+    </row>
+    <row r="75">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="8"/>
+      <c r="E75" s="1"/>
+      <c r="I75" s="1"/>
+      <c r="K75" s="1"/>
+      <c r="L75" s="1"/>
+      <c r="M75" s="1"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="R75" s="1"/>
+      <c r="S75" s="1"/>
+      <c r="T75" s="1"/>
+      <c r="U75" s="1"/>
+      <c r="V75" s="1"/>
+      <c r="AK75" s="1"/>
+      <c r="AL75" s="1"/>
+    </row>
+    <row r="76">
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="9"/>
+      <c r="G76" s="9"/>
+      <c r="H76" s="9"/>
+      <c r="I76" s="1"/>
+    </row>
+    <row r="77">
+      <c r="D77" s="2"/>
+      <c r="E77" s="2"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="9"/>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+    </row>
+    <row r="78">
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="9"/>
+      <c r="G78" s="9"/>
+    </row>
+    <row r="79">
+      <c r="E79" s="1"/>
+      <c r="F79" s="9"/>
+    </row>
+    <row r="80">
+      <c r="E80" s="1"/>
+      <c r="F80" s="9"/>
+    </row>
+    <row r="81">
+      <c r="E81" s="1"/>
+      <c r="F81" s="9"/>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>